<commit_message>
fix: Data has be sending to SE
The problem with a envelope soap is debuged
</commit_message>
<xml_diff>
--- a/Entrevista de Desligamento.xlsx
+++ b/Entrevista de Desligamento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinzen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\ProjectFormSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{AD74628D-BE06-4FC1-BE04-2187DD70E9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52976C5D-E81C-413D-9AE9-21DE5EC51D9A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63FFE92-6080-46EA-8844-0E7DBB28E646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
   <si>
     <t>Id</t>
   </si>
@@ -219,13 +219,16 @@
   </si>
   <si>
     <t>Sim</t>
+  </si>
+  <si>
+    <t>Adriano</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1165,15 +1168,15 @@
   <dimension ref="A1:BA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="53" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:53">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1351,7 +1354,7 @@
         <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G2" s="1">
         <v>45536</v>

</xml_diff>

<commit_message>
bug: the code execute but has a error
An error occurred: ('Connection aborted.', RemoteDisconnected('Remote end closed connection without response'))
</commit_message>
<xml_diff>
--- a/Entrevista de Desligamento.xlsx
+++ b/Entrevista de Desligamento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\ProjectFormSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinzen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63FFE92-6080-46EA-8844-0E7DBB28E646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{AD74628D-BE06-4FC1-BE04-2187DD70E9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08CEA3AC-04FA-4C2B-B87D-D311EE8BF336}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="77">
   <si>
     <t>Id</t>
   </si>
@@ -56,6 +56,9 @@
     <t>Nome completo</t>
   </si>
   <si>
+    <t>Data de Admissão</t>
+  </si>
+  <si>
     <t>Data de Demissão</t>
   </si>
   <si>
@@ -89,7 +92,7 @@
     <t>Demais considerações referente a sua avaliação acima2</t>
   </si>
   <si>
-    <t>Como você avalia os benefícios oferecidos pela empresa</t>
+    <t>Como você avalia o ambiente de trabalho, clima e relacionamentos no seu setor</t>
   </si>
   <si>
     <t>Vale Transporte</t>
@@ -149,9 +152,6 @@
     <t>Demais considerações referente a sua avaliação acima:3</t>
   </si>
   <si>
-    <t>Como você avalia os Programas e Ações direcionadas para o colaborador</t>
-  </si>
-  <si>
     <t>Comunicação Interna ¨Vem com o RH"; "Vem  Conferir"</t>
   </si>
   <si>
@@ -197,38 +197,83 @@
     <t>Qual mensagem você gostaria de deixar para a FGM?</t>
   </si>
   <si>
-    <t>adriano.guerra@fgmdentalgroup.com</t>
-  </si>
-  <si>
-    <t>Adriano Elsenbach Guerra</t>
+    <t>anonymous</t>
+  </si>
+  <si>
+    <t>JhonnyAnthony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rh </t>
+  </si>
+  <si>
+    <t>analista</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>bonito demais</t>
+  </si>
+  <si>
+    <t>1. Excelente</t>
+  </si>
+  <si>
+    <t>2. Bom</t>
+  </si>
+  <si>
+    <t>5. Não Utilizado</t>
+  </si>
+  <si>
+    <t>4. Ruim</t>
+  </si>
+  <si>
+    <t>3. Regular</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>anônima</t>
+  </si>
+  <si>
+    <t>Adriano</t>
+  </si>
+  <si>
+    <t>TI</t>
   </si>
   <si>
     <t>Teste</t>
   </si>
   <si>
-    <t>Empresa</t>
-  </si>
-  <si>
-    <t>1. Excelente</t>
-  </si>
-  <si>
-    <t>teste</t>
-  </si>
-  <si>
-    <t>Opção 11. Excelente</t>
-  </si>
-  <si>
-    <t>Sim</t>
-  </si>
-  <si>
-    <t>Adriano</t>
+    <t>Aniel Osta Ruger</t>
+  </si>
+  <si>
+    <t>Tecnologia de Empilhadeiras</t>
+  </si>
+  <si>
+    <t>Analista de empilhadeiras</t>
+  </si>
+  <si>
+    <t>Colaborador</t>
+  </si>
+  <si>
+    <t>Tava querendo pah</t>
+  </si>
+  <si>
+    <t>Jonas</t>
+  </si>
+  <si>
+    <t>Bomboclat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,18 +302,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
+  <dxfs count="49">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -430,10 +474,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:BA2" totalsRowShown="0">
-  <autoFilter ref="A1:BA2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:BA4" totalsRowShown="0">
+  <autoFilter ref="A1:BA4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="53">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="49">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="48">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="id"/>
@@ -454,248 +498,248 @@
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="48">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="47">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="responder"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nome" dataDxfId="47">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nome" dataDxfId="46">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="responderName"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nome completo" dataDxfId="46">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nome completo" dataDxfId="45">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rb6a547770f3149eba2a7f1fbce64248e"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Data de Demissão">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Data de Admissão">
+      <extLst>
+        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
+          <xlmsforms:question id="r13291b3c68ec41adae23da411e5c6b39"/>
+        </ext>
+      </extLst>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Data de Demissão">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r4f9d9e9310ab47c6abd501aef9b58e6e"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Setor" dataDxfId="45">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Setor" dataDxfId="44">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rc386fabfa6284f2583d9712eb4fe4516"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Cargo" dataDxfId="44">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Cargo" dataDxfId="43">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r4d75d3e176bb4ddbbec82661869e18e0"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Iniciativa do Desligamento" dataDxfId="43">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Iniciativa do Desligamento" dataDxfId="42">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r196ec82e910247ceb21fe4af03a6e929"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Quais foram os motivos que o levaram a solicitar seu Desligamento" dataDxfId="42">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Quais foram os motivos que o levaram a solicitar seu Desligamento" dataDxfId="41">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r24b041cf617649bf8ec257fc8a276c12"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="De maneira geral como você avalia sua jornada na FGM" dataDxfId="41">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="De maneira geral como você avalia sua jornada na FGM" dataDxfId="40">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="re7c35ffd867042dda50a5379e572afea"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Demais considerações referente a sua avaliação acima" dataDxfId="40">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Demais considerações referente a sua avaliação acima" dataDxfId="39">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r5b76d9500e53451898651b96a11c405d"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Como você avalia a estrutura da FGM (áreas internas e local de trabalho):" dataDxfId="39">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Como você avalia a estrutura da FGM (áreas internas e local de trabalho):" dataDxfId="38">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r8bee105823d640abbc77a33b4a2df7ef"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Demais considerações referente a sua avaliação acima1" dataDxfId="38">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Demais considerações referente a sua avaliação acima1" dataDxfId="37">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r4696c4622da1493e8834bf7e93ed7e70"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Como você avalia o ambiente de trabalho, clima e relacionamentos dentro da empresa" dataDxfId="37">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Como você avalia o ambiente de trabalho, clima e relacionamentos dentro da empresa" dataDxfId="36">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rc45aded9c6ec4365ab53fa51091c041c"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Demais considerações referente a sua avaliação acima2" dataDxfId="36">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Demais considerações referente a sua avaliação acima2" dataDxfId="35">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="raf7d459c3469414082c73cfadcbbb4b2"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Como você avalia os benefícios oferecidos pela empresa" dataDxfId="35">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="rf668d868752443a49076618020cb8aff"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Vale Transporte" dataDxfId="34">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Como você avalia o ambiente de trabalho, clima e relacionamentos no seu setor" dataDxfId="34">
+      <extLst>
+        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
+          <xlmsforms:question id="r4f488e54755d4a89bbf5bf59bbca1d5c"/>
+        </ext>
+      </extLst>
+    </tableColumn>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Vale Transporte" dataDxfId="33">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="re6f84ba3f8b3413e9c25f573edfa34f9"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Vale Refeição ou Restaurante" dataDxfId="33">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Vale Refeição ou Restaurante" dataDxfId="32">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r7b812024c3f8401a8a7ca9129dc3e01d"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Plano de Saúde Médico" dataDxfId="32">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Plano de Saúde Médico" dataDxfId="31">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r99d621de83414eb1a32bb75d1aaa5ca2"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Plano de Saúde Odontológico" dataDxfId="31">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Plano de Saúde Odontológico" dataDxfId="30">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rd38a2ed654b04ee3a09ea6c0ec70d139"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Convênio Farmácia Sesi" dataDxfId="30">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Convênio Farmácia Sesi" dataDxfId="29">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r0d51f1f5784d46c0b87ba9777e53d3bb"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Convênio Sesi Odonto" dataDxfId="29">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Convênio Sesi Odonto" dataDxfId="28">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r76991b903bb74f1dbd7aa24f2b6a38ad"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Presente Aniversário" dataDxfId="28">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Presente Aniversário" dataDxfId="27">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r7e76e1868bed4787a70629ad2a3b19d5"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Presente Casamento" dataDxfId="27">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Presente Casamento" dataDxfId="26">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rcc845650fbc1426a80a2750a2a8fcc50"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Presente Nascimento" dataDxfId="26">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Presente Nascimento" dataDxfId="25">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r448d61f5be9649fd86875cca856b8705"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Vacina Contra a Gripe" dataDxfId="25">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Vacina Contra a Gripe" dataDxfId="24">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r6213f43e045c4c05b01bb74748165254"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Seguro de Vida" dataDxfId="24">
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Seguro de Vida" dataDxfId="23">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rd19ef7ebfeb848789d3f17ed362a6783"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Bolsa de Estudo" dataDxfId="23">
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Bolsa de Estudo" dataDxfId="22">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rc0a6c9d883c549a6b2339bdd4eb70cf0"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Demais considerações referente a sua avaliação acima:" dataDxfId="22">
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Demais considerações referente a sua avaliação acima:" dataDxfId="21">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r42c072ad8718457fa71658c22bfe0d73"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Como você avalia a sua atuação no cargo que exercia, suas responsabilidades, entregas e o seu desenvolvimento profissional na FGM" dataDxfId="21">
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Como você avalia a sua atuação no cargo que exercia, suas responsabilidades, entregas e o seu desenvolvimento profissional na FGM" dataDxfId="20">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r860fdbf4d6564ee9bc6477cae173e98b"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Demais considerações referente a sua avaliação acima:1" dataDxfId="20">
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Demais considerações referente a sua avaliação acima:1" dataDxfId="19">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r232c9ac39d0f43899dc755b36a672fb5"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Como você avalia os recursos disponibilizados para você realizar o seu trabalho (sistema, notebook, celular, carro, demais recursos)" dataDxfId="19">
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Como você avalia os recursos disponibilizados para você realizar o seu trabalho (sistema, notebook, celular, carro, demais recursos)" dataDxfId="18">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r32d0957b606e406eb86a93073573d929"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Demais considerações referente a sua avaliação acima:2" dataDxfId="18">
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Demais considerações referente a sua avaliação acima:2" dataDxfId="17">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r20a01364b6114736b80e4c3ab89312ba"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Como você avalia a sua gestão direta - gestor(a), prestava suporte e direcionamentos necessários para você realizar suas atividades, exercia efetivamente a Liderança no setor" dataDxfId="17">
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Como você avalia a sua gestão direta - gestor(a), prestava suporte e direcionamentos necessários para você realizar suas atividades, exercia efetivamente a Liderança no setor" dataDxfId="16">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r5fcfbe6ac9444ad6b3118d61cc1e55b8"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Demais considerações referente a sua avaliação acima:3" dataDxfId="16">
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Demais considerações referente a sua avaliação acima:3" dataDxfId="15">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r4111aede73f846b1adcf05ace3037f7a"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Como você avalia os Programas e Ações direcionadas para o colaborador" dataDxfId="15">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="r07182c8ed3c44e20bd2b68b25902f1dc"/>
         </ext>
       </extLst>
     </tableColumn>
@@ -808,13 +852,14 @@
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{839C7E11-91E4-4DBD-9C5D-0DEA604FA9AC}">
-      <xlmsforms:msForm id="adMg4qjmJkGD77S2u_2TZz69AtZSZ0pLncDHq2Ag8tNUM1ZBQkFZVUFCMEYyNEM0SDJFNUhUTDZBUS4u" maxResponseId="1" latestEventMarker="0">
+      <xlmsforms:msForm id="adMg4qjmJkGD77S2u_2TZz69AtZSZ0pLncDHq2Ag8tNUM1ZBQkFZVUFCMEYyNEM0SDJFNUhUTDZBUS4u" isFormConnected="1" maxResponseId="5" latestEventMarker="16">
         <xlmsforms:syncedQuestionId>id</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>startDate</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>submitDate</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>responder</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>responderName</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>rb6a547770f3149eba2a7f1fbce64248e</xlmsforms:syncedQuestionId>
+        <xlmsforms:syncedQuestionId>r13291b3c68ec41adae23da411e5c6b39</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r4f9d9e9310ab47c6abd501aef9b58e6e</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>rc386fabfa6284f2583d9712eb4fe4516</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r4d75d3e176bb4ddbbec82661869e18e0</xlmsforms:syncedQuestionId>
@@ -826,7 +871,7 @@
         <xlmsforms:syncedQuestionId>r4696c4622da1493e8834bf7e93ed7e70</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>rc45aded9c6ec4365ab53fa51091c041c</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>raf7d459c3469414082c73cfadcbbb4b2</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rf668d868752443a49076618020cb8aff</xlmsforms:syncedQuestionId>
+        <xlmsforms:syncedQuestionId>r4f488e54755d4a89bbf5bf59bbca1d5c</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>re6f84ba3f8b3413e9c25f573edfa34f9</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r7b812024c3f8401a8a7ca9129dc3e01d</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r99d621de83414eb1a32bb75d1aaa5ca2</xlmsforms:syncedQuestionId>
@@ -846,7 +891,6 @@
         <xlmsforms:syncedQuestionId>r20a01364b6114736b80e4c3ab89312ba</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r5fcfbe6ac9444ad6b3118d61cc1e55b8</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r4111aede73f846b1adcf05ace3037f7a</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r07182c8ed3c44e20bd2b68b25902f1dc</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r811bc94aee01401cb05ba7653c561d79</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r0c62a7505d844732a6020b7a47ef7c5b</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>rc12c396c7230461ba8182b58e23fea59</xlmsforms:syncedQuestionId>
@@ -1165,18 +1209,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA2"/>
+  <dimension ref="A1:BA4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="53" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:53">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1337,30 +1381,27 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>45561.422824074078</v>
+        <v>45582.484525462962</v>
       </c>
       <c r="C2" s="2">
-        <v>45561.424467592595</v>
+        <v>45582.485821759263</v>
       </c>
       <c r="D2" t="s">
         <v>53</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>54</v>
       </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
       <c r="G2" s="1">
-        <v>45536</v>
-      </c>
-      <c r="H2" t="s">
-        <v>55</v>
+        <v>45580</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45586</v>
       </c>
       <c r="I2" t="s">
         <v>55</v>
@@ -1369,133 +1410,401 @@
         <v>56</v>
       </c>
       <c r="K2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" t="s">
+        <v>60</v>
+      </c>
+      <c r="T2" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" t="s">
+        <v>59</v>
+      </c>
+      <c r="V2" t="s">
+        <v>59</v>
+      </c>
+      <c r="W2" t="s">
+        <v>59</v>
+      </c>
+      <c r="X2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45582.499583333301</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45582.500798611101</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45589</v>
+      </c>
+      <c r="H3" s="1">
+        <v>45569</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O2" t="s">
-        <v>58</v>
-      </c>
-      <c r="P2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>58</v>
-      </c>
-      <c r="R2" t="s">
-        <v>58</v>
-      </c>
-      <c r="S2" t="s">
-        <v>57</v>
-      </c>
-      <c r="T2" t="s">
-        <v>57</v>
-      </c>
-      <c r="U2" t="s">
-        <v>57</v>
-      </c>
-      <c r="V2" t="s">
-        <v>57</v>
-      </c>
-      <c r="W2" t="s">
-        <v>57</v>
-      </c>
-      <c r="X2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AW2" t="s">
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AW3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AX3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AZ3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="BA3" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53">
+      <c r="A4" s="4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45582.483807870398</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45582.5441319444</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="1">
+        <v>45321</v>
+      </c>
+      <c r="H4" s="1">
+        <v>45540</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AX2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AY2" t="s">
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AZ2" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>58</v>
+      <c r="U4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV4" s="3"/>
+      <c r="AW4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AX4" s="3"/>
+      <c r="AY4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AZ4" s="3"/>
+      <c r="BA4" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BUG: I find where the bug is
test if is because daniel create a forms or not
</commit_message>
<xml_diff>
--- a/Entrevista de Desligamento.xlsx
+++ b/Entrevista de Desligamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\ProjectFormSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63FFE92-6080-46EA-8844-0E7DBB28E646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B292475-48CA-420C-B72F-A8F8CC6FB8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="80">
   <si>
     <t>Id</t>
   </si>
@@ -56,6 +56,9 @@
     <t>Nome completo</t>
   </si>
   <si>
+    <t>Data de Admissão</t>
+  </si>
+  <si>
     <t>Data de Demissão</t>
   </si>
   <si>
@@ -89,7 +92,10 @@
     <t>Demais considerações referente a sua avaliação acima2</t>
   </si>
   <si>
-    <t>Como você avalia os benefícios oferecidos pela empresa</t>
+    <t>Como você avalia o ambiente de trabalho, clima e relacionamentos no seu setor</t>
+  </si>
+  <si>
+    <t>Demais considerações referente a sua avaliação acima3</t>
   </si>
   <si>
     <t>Vale Transporte</t>
@@ -149,9 +155,6 @@
     <t>Demais considerações referente a sua avaliação acima:3</t>
   </si>
   <si>
-    <t>Como você avalia os Programas e Ações direcionadas para o colaborador</t>
-  </si>
-  <si>
     <t>Comunicação Interna ¨Vem com o RH"; "Vem  Conferir"</t>
   </si>
   <si>
@@ -179,57 +182,116 @@
     <t>Onboarding (Admissão e Integração na empresa)</t>
   </si>
   <si>
-    <t>Demais considerações referente a sua avaliação acima3</t>
+    <t>Demais considerações referente a sua avaliação acima4</t>
   </si>
   <si>
     <t>Você voltaria a trabalhar na FGM</t>
   </si>
   <si>
-    <t>Demais considerações referente a sua avaliação acima4</t>
+    <t>Demais considerações referente a sua avaliação acima5</t>
   </si>
   <si>
     <t>Você indicaria a FGM para alguém</t>
   </si>
   <si>
-    <t>Demais considerações referente a sua avaliação acima5</t>
+    <t>Demais considerações referente a sua avaliação acima6</t>
   </si>
   <si>
     <t>Qual mensagem você gostaria de deixar para a FGM?</t>
   </si>
   <si>
-    <t>adriano.guerra@fgmdentalgroup.com</t>
-  </si>
-  <si>
-    <t>Adriano Elsenbach Guerra</t>
-  </si>
-  <si>
-    <t>Teste</t>
-  </si>
-  <si>
-    <t>Empresa</t>
+    <t>anonymous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ronaldinho </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expedição </t>
+  </si>
+  <si>
+    <t>Empilhadeira</t>
+  </si>
+  <si>
+    <t>Colaborador</t>
+  </si>
+  <si>
+    <t>jogar a copa</t>
   </si>
   <si>
     <t>1. Excelente</t>
   </si>
   <si>
-    <t>teste</t>
-  </si>
-  <si>
-    <t>Opção 11. Excelente</t>
+    <t>2. Bom</t>
+  </si>
+  <si>
+    <t>3. Regular</t>
+  </si>
+  <si>
+    <t>bem top</t>
+  </si>
+  <si>
+    <t>4. Ruim</t>
+  </si>
+  <si>
+    <t>5. Não Utilizado</t>
   </si>
   <si>
     <t>Sim</t>
   </si>
   <si>
-    <t>Adriano</t>
+    <t>Não</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siirre </t>
+  </si>
+  <si>
+    <t>anônima</t>
+  </si>
+  <si>
+    <t>Carlos Drummond</t>
+  </si>
+  <si>
+    <t>Livraria</t>
+  </si>
+  <si>
+    <t>Escritor</t>
+  </si>
+  <si>
+    <t>Não queria trabalhar</t>
+  </si>
+  <si>
+    <t>Massa</t>
+  </si>
+  <si>
+    <t>Estua</t>
+  </si>
+  <si>
+    <t>daora</t>
+  </si>
+  <si>
+    <t>Esclerose</t>
+  </si>
+  <si>
+    <t>romario</t>
+  </si>
+  <si>
+    <t>Futebol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -257,10 +319,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,9 +497,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:BA2" totalsRowShown="0">
-  <autoFilter ref="A1:BA2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:BB3" totalsRowShown="0">
+  <autoFilter ref="A1:BB3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="54">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="49">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
@@ -475,329 +542,336 @@
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Data de Demissão">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Data de Admissão">
+      <extLst>
+        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
+          <xlmsforms:question id="r13291b3c68ec41adae23da411e5c6b39"/>
+        </ext>
+      </extLst>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Data de Demissão">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r4f9d9e9310ab47c6abd501aef9b58e6e"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Setor" dataDxfId="45">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Setor" dataDxfId="45">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rc386fabfa6284f2583d9712eb4fe4516"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Cargo" dataDxfId="44">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Cargo" dataDxfId="44">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r4d75d3e176bb4ddbbec82661869e18e0"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Iniciativa do Desligamento" dataDxfId="43">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Iniciativa do Desligamento" dataDxfId="43">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r196ec82e910247ceb21fe4af03a6e929"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Quais foram os motivos que o levaram a solicitar seu Desligamento" dataDxfId="42">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Quais foram os motivos que o levaram a solicitar seu Desligamento" dataDxfId="42">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r24b041cf617649bf8ec257fc8a276c12"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="De maneira geral como você avalia sua jornada na FGM" dataDxfId="41">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="De maneira geral como você avalia sua jornada na FGM" dataDxfId="41">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="re7c35ffd867042dda50a5379e572afea"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Demais considerações referente a sua avaliação acima" dataDxfId="40">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Demais considerações referente a sua avaliação acima" dataDxfId="40">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r5b76d9500e53451898651b96a11c405d"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Como você avalia a estrutura da FGM (áreas internas e local de trabalho):" dataDxfId="39">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Como você avalia a estrutura da FGM (áreas internas e local de trabalho):" dataDxfId="39">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r8bee105823d640abbc77a33b4a2df7ef"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Demais considerações referente a sua avaliação acima1" dataDxfId="38">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Demais considerações referente a sua avaliação acima1" dataDxfId="38">
+      <extLst>
+        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
+          <xlmsforms:question id="r53a3c50a40ee434da7f16b7e9fbb9db6"/>
+        </ext>
+      </extLst>
+    </tableColumn>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Como você avalia o ambiente de trabalho, clima e relacionamentos dentro da empresa" dataDxfId="37">
+      <extLst>
+        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
+          <xlmsforms:question id="rc45aded9c6ec4365ab53fa51091c041c"/>
+        </ext>
+      </extLst>
+    </tableColumn>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Demais considerações referente a sua avaliação acima2" dataDxfId="36">
+      <extLst>
+        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
+          <xlmsforms:question id="r26197fa767d44d8f96c60c13741ead6e"/>
+        </ext>
+      </extLst>
+    </tableColumn>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Como você avalia o ambiente de trabalho, clima e relacionamentos no seu setor" dataDxfId="35">
+      <extLst>
+        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
+          <xlmsforms:question id="r4f488e54755d4a89bbf5bf59bbca1d5c"/>
+        </ext>
+      </extLst>
+    </tableColumn>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Demais considerações referente a sua avaliação acima3" dataDxfId="34">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r4696c4622da1493e8834bf7e93ed7e70"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Como você avalia o ambiente de trabalho, clima e relacionamentos dentro da empresa" dataDxfId="37">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="rc45aded9c6ec4365ab53fa51091c041c"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Demais considerações referente a sua avaliação acima2" dataDxfId="36">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="raf7d459c3469414082c73cfadcbbb4b2"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Como você avalia os benefícios oferecidos pela empresa" dataDxfId="35">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="rf668d868752443a49076618020cb8aff"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Vale Transporte" dataDxfId="34">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Vale Transporte" dataDxfId="33">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="re6f84ba3f8b3413e9c25f573edfa34f9"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Vale Refeição ou Restaurante" dataDxfId="33">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Vale Refeição ou Restaurante" dataDxfId="32">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r7b812024c3f8401a8a7ca9129dc3e01d"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Plano de Saúde Médico" dataDxfId="32">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Plano de Saúde Médico" dataDxfId="31">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r99d621de83414eb1a32bb75d1aaa5ca2"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Plano de Saúde Odontológico" dataDxfId="31">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Plano de Saúde Odontológico" dataDxfId="30">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rd38a2ed654b04ee3a09ea6c0ec70d139"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Convênio Farmácia Sesi" dataDxfId="30">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Convênio Farmácia Sesi" dataDxfId="29">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r0d51f1f5784d46c0b87ba9777e53d3bb"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Convênio Sesi Odonto" dataDxfId="29">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Convênio Sesi Odonto" dataDxfId="28">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r76991b903bb74f1dbd7aa24f2b6a38ad"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Presente Aniversário" dataDxfId="28">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Presente Aniversário" dataDxfId="27">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r7e76e1868bed4787a70629ad2a3b19d5"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Presente Casamento" dataDxfId="27">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Presente Casamento" dataDxfId="26">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rcc845650fbc1426a80a2750a2a8fcc50"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Presente Nascimento" dataDxfId="26">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Presente Nascimento" dataDxfId="25">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r448d61f5be9649fd86875cca856b8705"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Vacina Contra a Gripe" dataDxfId="25">
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Vacina Contra a Gripe" dataDxfId="24">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r6213f43e045c4c05b01bb74748165254"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Seguro de Vida" dataDxfId="24">
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Seguro de Vida" dataDxfId="23">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rd19ef7ebfeb848789d3f17ed362a6783"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Bolsa de Estudo" dataDxfId="23">
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Bolsa de Estudo" dataDxfId="22">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rc0a6c9d883c549a6b2339bdd4eb70cf0"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Demais considerações referente a sua avaliação acima:" dataDxfId="22">
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Demais considerações referente a sua avaliação acima:" dataDxfId="21">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r42c072ad8718457fa71658c22bfe0d73"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Como você avalia a sua atuação no cargo que exercia, suas responsabilidades, entregas e o seu desenvolvimento profissional na FGM" dataDxfId="21">
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Como você avalia a sua atuação no cargo que exercia, suas responsabilidades, entregas e o seu desenvolvimento profissional na FGM" dataDxfId="20">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r860fdbf4d6564ee9bc6477cae173e98b"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Demais considerações referente a sua avaliação acima:1" dataDxfId="20">
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Demais considerações referente a sua avaliação acima:1" dataDxfId="19">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r232c9ac39d0f43899dc755b36a672fb5"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Como você avalia os recursos disponibilizados para você realizar o seu trabalho (sistema, notebook, celular, carro, demais recursos)" dataDxfId="19">
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Como você avalia os recursos disponibilizados para você realizar o seu trabalho (sistema, notebook, celular, carro, demais recursos)" dataDxfId="18">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r32d0957b606e406eb86a93073573d929"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Demais considerações referente a sua avaliação acima:2" dataDxfId="18">
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Demais considerações referente a sua avaliação acima:2" dataDxfId="17">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r20a01364b6114736b80e4c3ab89312ba"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Como você avalia a sua gestão direta - gestor(a), prestava suporte e direcionamentos necessários para você realizar suas atividades, exercia efetivamente a Liderança no setor" dataDxfId="17">
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Como você avalia a sua gestão direta - gestor(a), prestava suporte e direcionamentos necessários para você realizar suas atividades, exercia efetivamente a Liderança no setor" dataDxfId="16">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r5fcfbe6ac9444ad6b3118d61cc1e55b8"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Demais considerações referente a sua avaliação acima:3" dataDxfId="16">
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Demais considerações referente a sua avaliação acima:3" dataDxfId="15">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r4111aede73f846b1adcf05ace3037f7a"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Como você avalia os Programas e Ações direcionadas para o colaborador" dataDxfId="15">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="r07182c8ed3c44e20bd2b68b25902f1dc"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Comunicação Interna ¨Vem com o RH&quot;; &quot;Vem  Conferir&quot;" dataDxfId="14">
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Comunicação Interna ¨Vem com o RH&quot;; &quot;Vem  Conferir&quot;" dataDxfId="14">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r811bc94aee01401cb05ba7653c561d79"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Endomarketing (Comemorações e Eventos Internos)" dataDxfId="13">
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Endomarketing (Comemorações e Eventos Internos)" dataDxfId="13">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r0c62a7505d844732a6020b7a47ef7c5b"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Treinamento e Desenvolvimento Profissional" dataDxfId="12">
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Treinamento e Desenvolvimento Profissional" dataDxfId="12">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rc12c396c7230461ba8182b58e23fea59"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Recrutamento Interno" dataDxfId="11">
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Recrutamento Interno" dataDxfId="11">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r0ab79cbb23834110a709fd32be8fbfef"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Suporte para Folha de Pagamento e Benefícios" dataDxfId="10">
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Suporte para Folha de Pagamento e Benefícios" dataDxfId="10">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rb2f8a78f10a743128d4f713fa023bc04"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Segurança do Trabalho" dataDxfId="9">
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="Segurança do Trabalho" dataDxfId="9">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r193f01ae13ce4540bf0adfe0a4cae37f"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="Canal de Ouvidoria" dataDxfId="8">
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="Canal de Ouvidoria" dataDxfId="8">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r31de4726e2254567b76b766c136187cf"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="CCQ" dataDxfId="7">
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="CCQ" dataDxfId="7">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rcb869d56231a4102a6e54e498567d689"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="Onboarding (Admissão e Integração na empresa)" dataDxfId="6">
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="Onboarding (Admissão e Integração na empresa)" dataDxfId="6">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rafc50f4526b54766bf91723ece0a6ac7"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="Demais considerações referente a sua avaliação acima3" dataDxfId="5">
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="Demais considerações referente a sua avaliação acima4" dataDxfId="5">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="raaca2264129c49088fb2690af3ff2546"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="Você voltaria a trabalhar na FGM" dataDxfId="4">
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="Você voltaria a trabalhar na FGM" dataDxfId="4">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r031da7b045344967b5dbbba2c20bd577"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="Demais considerações referente a sua avaliação acima4" dataDxfId="3">
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="Demais considerações referente a sua avaliação acima5" dataDxfId="3">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r2b3e2a0152f84040bc4fe698c28f989b"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="Você indicaria a FGM para alguém" dataDxfId="2">
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="Você indicaria a FGM para alguém" dataDxfId="2">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r0c05cae0fa7b4a438efc5fc272890f21"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="Demais considerações referente a sua avaliação acima5" dataDxfId="1">
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="Demais considerações referente a sua avaliação acima6" dataDxfId="1">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rfaec55be0c3244f38c2d3b83193013cd"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="Qual mensagem você gostaria de deixar para a FGM?" dataDxfId="0">
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="Qual mensagem você gostaria de deixar para a FGM?" dataDxfId="0">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r72d5c7b254824d048a87827ab4e930ea"/>
@@ -808,13 +882,14 @@
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{839C7E11-91E4-4DBD-9C5D-0DEA604FA9AC}">
-      <xlmsforms:msForm id="adMg4qjmJkGD77S2u_2TZz69AtZSZ0pLncDHq2Ag8tNUM1ZBQkFZVUFCMEYyNEM0SDJFNUhUTDZBUS4u" maxResponseId="1" latestEventMarker="0">
+      <xlmsforms:msForm id="adMg4qjmJkGD77S2u_2TZz69AtZSZ0pLncDHq2Ag8tNUM1ZBQkFZVUFCMEYyNEM0SDJFNUhUTDZBUS4u" isFormConnected="1" maxResponseId="10" latestEventMarker="32">
         <xlmsforms:syncedQuestionId>id</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>startDate</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>submitDate</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>responder</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>responderName</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>rb6a547770f3149eba2a7f1fbce64248e</xlmsforms:syncedQuestionId>
+        <xlmsforms:syncedQuestionId>r13291b3c68ec41adae23da411e5c6b39</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r4f9d9e9310ab47c6abd501aef9b58e6e</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>rc386fabfa6284f2583d9712eb4fe4516</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r4d75d3e176bb4ddbbec82661869e18e0</xlmsforms:syncedQuestionId>
@@ -823,10 +898,11 @@
         <xlmsforms:syncedQuestionId>re7c35ffd867042dda50a5379e572afea</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r5b76d9500e53451898651b96a11c405d</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r8bee105823d640abbc77a33b4a2df7ef</xlmsforms:syncedQuestionId>
+        <xlmsforms:syncedQuestionId>r53a3c50a40ee434da7f16b7e9fbb9db6</xlmsforms:syncedQuestionId>
+        <xlmsforms:syncedQuestionId>rc45aded9c6ec4365ab53fa51091c041c</xlmsforms:syncedQuestionId>
+        <xlmsforms:syncedQuestionId>r26197fa767d44d8f96c60c13741ead6e</xlmsforms:syncedQuestionId>
+        <xlmsforms:syncedQuestionId>r4f488e54755d4a89bbf5bf59bbca1d5c</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r4696c4622da1493e8834bf7e93ed7e70</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rc45aded9c6ec4365ab53fa51091c041c</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>raf7d459c3469414082c73cfadcbbb4b2</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>rf668d868752443a49076618020cb8aff</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>re6f84ba3f8b3413e9c25f573edfa34f9</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r7b812024c3f8401a8a7ca9129dc3e01d</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r99d621de83414eb1a32bb75d1aaa5ca2</xlmsforms:syncedQuestionId>
@@ -846,7 +922,6 @@
         <xlmsforms:syncedQuestionId>r20a01364b6114736b80e4c3ab89312ba</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r5fcfbe6ac9444ad6b3118d61cc1e55b8</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r4111aede73f846b1adcf05ace3037f7a</xlmsforms:syncedQuestionId>
-        <xlmsforms:syncedQuestionId>r07182c8ed3c44e20bd2b68b25902f1dc</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r811bc94aee01401cb05ba7653c561d79</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>r0c62a7505d844732a6020b7a47ef7c5b</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>rc12c396c7230461ba8182b58e23fea59</xlmsforms:syncedQuestionId>
@@ -1165,18 +1240,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA2"/>
+  <dimension ref="A1:BB4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="53" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="54" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1336,166 +1411,455 @@
       <c r="BA1" t="s">
         <v>52</v>
       </c>
+      <c r="BB1" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
-        <v>45561.422824074078</v>
+        <v>45583.376759259256</v>
       </c>
       <c r="C2" s="2">
-        <v>45561.424467592595</v>
+        <v>45583.378692129627</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" t="s">
         <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G2" s="1">
-        <v>45536</v>
-      </c>
-      <c r="H2" t="s">
-        <v>55</v>
+        <v>36544</v>
+      </c>
+      <c r="H2" s="1">
+        <v>37419</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="O2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" t="s">
+        <v>65</v>
+      </c>
+      <c r="V2" t="s">
+        <v>60</v>
+      </c>
+      <c r="W2" t="s">
+        <v>61</v>
+      </c>
+      <c r="X2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5">
+        <v>45583.602476851898</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45583.6036805556</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="7">
+        <v>37803</v>
+      </c>
+      <c r="H3" s="7">
+        <v>45586</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="P2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="L3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AU3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="BA3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB3" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45583.558263888903</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45583.5603819444</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="1">
+        <v>45540</v>
+      </c>
+      <c r="H4" s="1">
+        <v>45572</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="R2" t="s">
-        <v>58</v>
-      </c>
-      <c r="S2" t="s">
-        <v>57</v>
-      </c>
-      <c r="T2" t="s">
-        <v>57</v>
-      </c>
-      <c r="U2" t="s">
-        <v>57</v>
-      </c>
-      <c r="V2" t="s">
-        <v>57</v>
-      </c>
-      <c r="W2" t="s">
-        <v>57</v>
-      </c>
-      <c r="X2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>58</v>
+      <c r="L4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AR4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW4" s="3"/>
+      <c r="AX4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY4" s="3"/>
+      <c r="AZ4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA4" s="3"/>
+      <c r="BB4" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: I fixed error with utf-8
I found how to declare a soap envelope with a UTF-8
</commit_message>
<xml_diff>
--- a/Entrevista de Desligamento.xlsx
+++ b/Entrevista de Desligamento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\ProjectFormSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinzen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B292475-48CA-420C-B72F-A8F8CC6FB8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{AD74628D-BE06-4FC1-BE04-2187DD70E9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64779057-20B7-4F2B-89AE-3780C31143F8}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -282,16 +282,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -319,15 +311,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,8 +486,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:BB3" totalsRowShown="0">
-  <autoFilter ref="A1:BB3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:BB4" totalsRowShown="0">
+  <autoFilter ref="A1:BB4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="54">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="49">
       <extLst>
@@ -1242,16 +1231,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="54" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1415,7 +1402,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54">
       <c r="A2">
         <v>8</v>
       </c>
@@ -1546,320 +1533,320 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+    <row r="3" spans="1:54">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45583.558263888903</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45583.5603819444</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45540</v>
+      </c>
+      <c r="H3" s="1">
+        <v>45572</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW3" s="3"/>
+      <c r="AX3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY3" s="3"/>
+      <c r="AZ3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA3" s="3"/>
+      <c r="BB3" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54">
+      <c r="A4" s="4">
         <v>10</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B4" s="2">
         <v>45583.602476851898</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C4" s="2">
         <v>45583.6036805556</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="7">
-        <v>37803</v>
-      </c>
-      <c r="H3" s="7">
-        <v>45586</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="W3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AS3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AT3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AU3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AV3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AW3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AX3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="BA3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="BB3" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2">
-        <v>45583.558263888903</v>
-      </c>
-      <c r="C4" s="2">
-        <v>45583.5603819444</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>69</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G4" s="1">
-        <v>45540</v>
+        <v>37803</v>
       </c>
       <c r="H4" s="1">
-        <v>45572</v>
+        <v>45586</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>58</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>60</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AC4" s="3" t="s">
         <v>62</v>
       </c>
       <c r="AD4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AF4" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="AG4" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="AH4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AI4" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AM4" s="3"/>
-      <c r="AN4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="AR4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AS4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AU4" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AV4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AW4" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="AW4" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="AX4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AY4" s="3"/>
+      <c r="AY4" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="AZ4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="BA4" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="BA4" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="BB4" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
buid: Just beauty modification
</commit_message>
<xml_diff>
--- a/Entrevista de Desligamento.xlsx
+++ b/Entrevista de Desligamento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinzen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\ProjectFormSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{AD74628D-BE06-4FC1-BE04-2187DD70E9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64779057-20B7-4F2B-89AE-3780C31143F8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699F7B76-5870-4E4A-938F-A20F4950B751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -282,8 +282,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -316,7 +324,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1231,14 +1239,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AV2" sqref="AV2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="54" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1402,7 +1412,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:54">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8</v>
       </c>
@@ -1520,8 +1530,8 @@
       <c r="AU2" t="s">
         <v>64</v>
       </c>
-      <c r="AV2" t="s">
-        <v>65</v>
+      <c r="AV2" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="AX2" t="s">
         <v>66</v>
@@ -1533,7 +1543,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:54">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9</v>
       </c>
@@ -1687,8 +1697,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:54">
-      <c r="A4" s="4">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>10</v>
       </c>
       <c r="B4" s="2">

</xml_diff>

<commit_message>
buid: Conection with db
</commit_message>
<xml_diff>
--- a/Entrevista de Desligamento.xlsx
+++ b/Entrevista de Desligamento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\ProjectFormSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinzen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699F7B76-5870-4E4A-938F-A20F4950B751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{AD74628D-BE06-4FC1-BE04-2187DD70E9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64779057-20B7-4F2B-89AE-3780C31143F8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -282,16 +282,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -324,7 +316,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1239,16 +1231,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="AV2" sqref="AV2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="54" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1412,7 +1402,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54">
       <c r="A2">
         <v>8</v>
       </c>
@@ -1530,8 +1520,8 @@
       <c r="AU2" t="s">
         <v>64</v>
       </c>
-      <c r="AV2" s="4" t="s">
-        <v>60</v>
+      <c r="AV2" t="s">
+        <v>65</v>
       </c>
       <c r="AX2" t="s">
         <v>66</v>
@@ -1543,7 +1533,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54">
       <c r="A3">
         <v>9</v>
       </c>
@@ -1697,8 +1687,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:54">
+      <c r="A4" s="4">
         <v>10</v>
       </c>
       <c r="B4" s="2">

</xml_diff>

<commit_message>
feat: Include logs to project
Logs are localizade all in Logs->Date
</commit_message>
<xml_diff>
--- a/Entrevista de Desligamento.xlsx
+++ b/Entrevista de Desligamento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28221"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinzen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{AD74628D-BE06-4FC1-BE04-2187DD70E9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64779057-20B7-4F2B-89AE-3780C31143F8}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{AD74628D-BE06-4FC1-BE04-2187DD70E9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE00DF10-0CFA-449E-916C-4AAC9E666C1A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="91">
   <si>
     <t>Id</t>
   </si>
@@ -276,14 +276,55 @@
   </si>
   <si>
     <t>Futebol</t>
+  </si>
+  <si>
+    <t>jhonny anthony de souza</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>ESTAGIARIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOGAR COPA </t>
+  </si>
+  <si>
+    <t>COPA DO MUNDO</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>JB</t>
+  </si>
+  <si>
+    <t>BJ</t>
+  </si>
+  <si>
+    <t>BJJB</t>
+  </si>
+  <si>
+    <t>JBJ</t>
+  </si>
+  <si>
+    <t>JBBJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -311,12 +352,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,8 +528,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:BB4" totalsRowShown="0">
-  <autoFilter ref="A1:BB4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:BB7" totalsRowShown="0">
+  <autoFilter ref="A1:BB7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="54">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="49">
       <extLst>
@@ -871,7 +913,7 @@
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{839C7E11-91E4-4DBD-9C5D-0DEA604FA9AC}">
-      <xlmsforms:msForm id="adMg4qjmJkGD77S2u_2TZz69AtZSZ0pLncDHq2Ag8tNUM1ZBQkFZVUFCMEYyNEM0SDJFNUhUTDZBUS4u" isFormConnected="1" maxResponseId="10" latestEventMarker="32">
+      <xlmsforms:msForm id="adMg4qjmJkGD77S2u_2TZz69AtZSZ0pLncDHq2Ag8tNUM1ZBQkFZVUFCMEYyNEM0SDJFNUhUTDZBUS4u" isFormConnected="1" maxResponseId="12" latestEventMarker="34">
         <xlmsforms:syncedQuestionId>id</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>startDate</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>submitDate</xlmsforms:syncedQuestionId>
@@ -1229,9 +1271,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BB4"/>
+  <dimension ref="A1:BB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AV6" activeCellId="1" sqref="AV2 AV6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1520,8 +1564,8 @@
       <c r="AU2" t="s">
         <v>64</v>
       </c>
-      <c r="AV2" t="s">
-        <v>65</v>
+      <c r="AV2" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="AX2" t="s">
         <v>66</v>
@@ -1688,7 +1732,7 @@
       </c>
     </row>
     <row r="4" spans="1:54">
-      <c r="A4" s="4">
+      <c r="A4">
         <v>10</v>
       </c>
       <c r="B4" s="2">
@@ -1847,6 +1891,385 @@
       </c>
       <c r="BB4" s="3" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45590.472523148099</v>
+      </c>
+      <c r="C5" s="2">
+        <v>45590.473738425899</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="1">
+        <v>37803</v>
+      </c>
+      <c r="H5" s="1">
+        <v>45590</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AU5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="BA5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB5" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+      <c r="AU6" s="3"/>
+      <c r="AV6" s="5"/>
+      <c r="AW6" s="3"/>
+      <c r="AX6" s="3"/>
+      <c r="AY6" s="3"/>
+      <c r="AZ6" s="3"/>
+      <c r="BA6" s="3"/>
+      <c r="BB6" s="3"/>
+    </row>
+    <row r="7" spans="1:54">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45590.475902777798</v>
+      </c>
+      <c r="C7" s="2">
+        <v>45590.477025462998</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="1">
+        <v>45589</v>
+      </c>
+      <c r="H7" s="1">
+        <v>45596</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AO7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AU7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AX7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AZ7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="BA7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="BB7" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>